<commit_message>
corretto l'errore per mancato accreditamento
Corretto l'errore
Con la presente si comunica il mancato superamento dei seguenti test [147] per il servizio [validazione/pubblicazione] del Fornitore [A1#111NOLEXXXXXXX] - Vendor:[Nolex] - ID: [NIGS] - Version: [2023.05.01.1200] - Sha: [f363d2722d8c6a1eb36aba49ee4d59924bdac862] in data odierna. 
"id" : 147,
  "error" : "MISSING_CLAIMS_ON_LOG_COLLECTOR",
  "description" : "Durante l'invocazione al gtw non è stato utilizzato un jwt con appId,appVersion,appVendor valorizzati"
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111NOLEXXXXXXX/Nolex/NIGS/2023.05.01.1200/report-checklist.xlsx
+++ b/GATEWAY/A1#111NOLEXXXXXXX/Nolex/NIGS/2023.05.01.1200/report-checklist.xlsx
@@ -761,15 +761,6 @@
     <t>connection Timeout</t>
   </si>
   <si>
-    <t>2023-05-16T13:48:04Z</t>
-  </si>
-  <si>
-    <t>f609ef3c427100a8</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.b6c509bc606895ed59d7b22eb303a149a0cb7654837da8fee76aa5b3681e9506.5f64152281^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2023-05-16T14:20:29Z</t>
   </si>
   <si>
@@ -977,6 +968,15 @@
   </si>
   <si>
     <t>Gestito in back office, l'operatore riesegue l'operazione dopo aver corretto l'errore.</t>
+  </si>
+  <si>
+    <t>2023-05-19T08:11:02Z</t>
+  </si>
+  <si>
+    <t>4606c5e69fcef404</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.b6c509bc606895ed59d7b22eb303a149a0cb7654837da8fee76aa5b3681e9506.e4f8134e1e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -3877,10 +3877,10 @@
   <dimension ref="A1:T652"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="P28" sqref="P28"/>
+      <selection pane="bottomRight" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4136,10 +4136,10 @@
         <v>45062</v>
       </c>
       <c r="G9" s="24" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H9" s="24" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="I9" s="24" t="s">
         <v>166</v>
@@ -4161,7 +4161,7 @@
         <v>60</v>
       </c>
       <c r="P9" s="25" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="Q9" s="25" t="s">
         <v>158</v>
@@ -4192,10 +4192,10 @@
         <v>45062</v>
       </c>
       <c r="G10" s="24" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="H10" s="24" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="I10" s="24" t="s">
         <v>166</v>
@@ -4217,7 +4217,7 @@
         <v>60</v>
       </c>
       <c r="P10" s="25" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="Q10" s="25" t="s">
         <v>158</v>
@@ -4263,7 +4263,7 @@
         <v>60</v>
       </c>
       <c r="P11" s="25" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="Q11" s="25" t="s">
         <v>158</v>
@@ -4296,13 +4296,13 @@
         <v>45062</v>
       </c>
       <c r="G12" s="24" t="s">
-        <v>171</v>
+        <v>232</v>
       </c>
       <c r="H12" s="24" t="s">
-        <v>172</v>
+        <v>233</v>
       </c>
       <c r="I12" s="24" t="s">
-        <v>173</v>
+        <v>234</v>
       </c>
       <c r="J12" s="25" t="s">
         <v>60</v>
@@ -4346,7 +4346,7 @@
         <v>160</v>
       </c>
       <c r="K13" s="25" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="L13" s="25"/>
       <c r="M13" s="25"/>
@@ -4386,7 +4386,7 @@
         <v>160</v>
       </c>
       <c r="K14" s="25" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="L14" s="25"/>
       <c r="M14" s="25"/>
@@ -4426,7 +4426,7 @@
         <v>160</v>
       </c>
       <c r="K15" s="25" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="L15" s="25"/>
       <c r="M15" s="25"/>
@@ -4462,13 +4462,13 @@
         <v>45062</v>
       </c>
       <c r="G16" s="24" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="H16" s="24" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="I16" s="24" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="J16" s="25" t="s">
         <v>60</v>
@@ -4481,13 +4481,13 @@
         <v>160</v>
       </c>
       <c r="N16" s="25" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="O16" s="25" t="s">
         <v>60</v>
       </c>
       <c r="P16" s="25" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="Q16" s="25" t="s">
         <v>158</v>
@@ -4518,13 +4518,13 @@
         <v>45062</v>
       </c>
       <c r="G17" s="24" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="H17" s="24" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="I17" s="24" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="J17" s="25" t="s">
         <v>60</v>
@@ -4537,13 +4537,13 @@
         <v>160</v>
       </c>
       <c r="N17" s="25" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="O17" s="25" t="s">
         <v>60</v>
       </c>
       <c r="P17" s="25" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="Q17" s="25" t="s">
         <v>158</v>
@@ -4574,13 +4574,13 @@
         <v>45062</v>
       </c>
       <c r="G18" s="24" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="H18" s="24" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="I18" s="24" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="J18" s="25" t="s">
         <v>60</v>
@@ -4593,13 +4593,13 @@
         <v>160</v>
       </c>
       <c r="N18" s="25" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="O18" s="25" t="s">
         <v>60</v>
       </c>
       <c r="P18" s="25" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="Q18" s="25" t="s">
         <v>158</v>
@@ -4630,13 +4630,13 @@
         <v>45062</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="H19" s="24" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="I19" s="24" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="J19" s="25" t="s">
         <v>60</v>
@@ -4649,13 +4649,13 @@
         <v>160</v>
       </c>
       <c r="N19" s="25" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="O19" s="25" t="s">
         <v>60</v>
       </c>
       <c r="P19" s="34" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="Q19" s="34" t="s">
         <v>158</v>
@@ -4686,13 +4686,13 @@
         <v>45062</v>
       </c>
       <c r="G20" s="33" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H20" s="33" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="I20" s="33" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="J20" s="34" t="s">
         <v>60</v>
@@ -4705,13 +4705,13 @@
         <v>160</v>
       </c>
       <c r="N20" s="34" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="O20" s="34" t="s">
         <v>60</v>
       </c>
       <c r="P20" s="34" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="Q20" s="34" t="s">
         <v>158</v>
@@ -4742,13 +4742,13 @@
         <v>45062</v>
       </c>
       <c r="G21" s="33" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="H21" s="33" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="I21" s="33" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="J21" s="34" t="s">
         <v>60</v>
@@ -4761,13 +4761,13 @@
         <v>160</v>
       </c>
       <c r="N21" s="34" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="O21" s="34" t="s">
         <v>60</v>
       </c>
       <c r="P21" s="34" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="Q21" s="34" t="s">
         <v>158</v>
@@ -4798,13 +4798,13 @@
         <v>45062</v>
       </c>
       <c r="G22" s="33" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H22" s="33" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="I22" s="33" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="J22" s="34" t="s">
         <v>60</v>
@@ -4817,13 +4817,13 @@
         <v>160</v>
       </c>
       <c r="N22" s="34" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="O22" s="34" t="s">
         <v>60</v>
       </c>
       <c r="P22" s="34" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="Q22" s="34" t="s">
         <v>158</v>
@@ -4854,13 +4854,13 @@
         <v>45062</v>
       </c>
       <c r="G23" s="33" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="H23" s="33" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="I23" s="33" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="J23" s="34" t="s">
         <v>60</v>
@@ -4873,13 +4873,13 @@
         <v>160</v>
       </c>
       <c r="N23" s="34" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="O23" s="34" t="s">
         <v>60</v>
       </c>
       <c r="P23" s="34" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="Q23" s="34" t="s">
         <v>158</v>
@@ -4910,13 +4910,13 @@
         <v>45062</v>
       </c>
       <c r="G24" s="33" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="H24" s="33" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="I24" s="33" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J24" s="34" t="s">
         <v>60</v>
@@ -4929,13 +4929,13 @@
         <v>160</v>
       </c>
       <c r="N24" s="34" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="O24" s="34" t="s">
         <v>60</v>
       </c>
       <c r="P24" s="34" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="Q24" s="34" t="s">
         <v>158</v>
@@ -4966,13 +4966,13 @@
         <v>45062</v>
       </c>
       <c r="G25" s="33" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="H25" s="33" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="I25" s="33" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J25" s="34" t="s">
         <v>60</v>
@@ -4985,13 +4985,13 @@
         <v>160</v>
       </c>
       <c r="N25" s="34" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="O25" s="34" t="s">
         <v>60</v>
       </c>
       <c r="P25" s="34" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="Q25" s="34" t="s">
         <v>158</v>
@@ -5022,13 +5022,13 @@
         <v>45062</v>
       </c>
       <c r="G26" s="33" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="H26" s="33" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="I26" s="33" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="J26" s="34" t="s">
         <v>60</v>
@@ -5041,13 +5041,13 @@
         <v>160</v>
       </c>
       <c r="N26" s="34" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="O26" s="34" t="s">
         <v>60</v>
       </c>
       <c r="P26" s="34" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="Q26" s="34" t="s">
         <v>158</v>
@@ -5082,7 +5082,7 @@
         <v>160</v>
       </c>
       <c r="K27" s="34" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="L27" s="25"/>
       <c r="M27" s="25"/>
@@ -5116,13 +5116,13 @@
         <v>45062</v>
       </c>
       <c r="G28" s="33" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="H28" s="33" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="I28" s="33" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="J28" s="34" t="s">
         <v>60</v>
@@ -5135,13 +5135,13 @@
         <v>160</v>
       </c>
       <c r="N28" s="34" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="O28" s="34" t="s">
         <v>60</v>
       </c>
       <c r="P28" s="34" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="Q28" s="34" t="s">
         <v>158</v>
@@ -5176,7 +5176,7 @@
         <v>160</v>
       </c>
       <c r="K29" s="34" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="L29" s="25"/>
       <c r="M29" s="25"/>
@@ -5214,7 +5214,7 @@
         <v>160</v>
       </c>
       <c r="K30" s="34" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="L30" s="25"/>
       <c r="M30" s="25"/>
@@ -5252,7 +5252,7 @@
         <v>160</v>
       </c>
       <c r="K31" s="34" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="L31" s="25"/>
       <c r="M31" s="25"/>
@@ -5290,7 +5290,7 @@
         <v>160</v>
       </c>
       <c r="K32" s="34" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="L32" s="25"/>
       <c r="M32" s="25"/>
@@ -5328,7 +5328,7 @@
         <v>160</v>
       </c>
       <c r="K33" s="34" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="L33" s="25"/>
       <c r="M33" s="25"/>
@@ -5362,13 +5362,13 @@
         <v>45062</v>
       </c>
       <c r="G34" s="33" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="H34" s="33" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="I34" s="33" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="J34" s="34" t="s">
         <v>60</v>
@@ -5381,13 +5381,13 @@
         <v>160</v>
       </c>
       <c r="N34" s="34" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="O34" s="34" t="s">
         <v>60</v>
       </c>
       <c r="P34" s="34" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="Q34" s="34" t="s">
         <v>158</v>

</xml_diff>

<commit_message>
Correzione per mancato accreditamento RSA
Casi :  ID [32, 40, 48, 151, 152, 153, 154, 155, 156, 157, 158, 159, 160, 161, 163, 169], rispetto a quanto riportato nella colonna “gestione errore”.
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111NOLEXXXXXXX/Nolex/NIGS/2023.05.01.1200/report-checklist.xlsx
+++ b/GATEWAY/A1#111NOLEXXXXXXX/Nolex/NIGS/2023.05.01.1200/report-checklist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="238">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -967,9 +967,6 @@
     <t>Le sezioni  non sono gestite dal software</t>
   </si>
   <si>
-    <t>Gestito in back office, l'operatore riesegue l'operazione dopo aver corretto l'errore.</t>
-  </si>
-  <si>
     <t>2023-05-19T08:11:02Z</t>
   </si>
   <si>
@@ -977,6 +974,38 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.150.4.4.b6c509bc606895ed59d7b22eb303a149a0cb7654837da8fee76aa5b3681e9506.e4f8134e1e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Viene gestito in back office.
+L'errore verrà corretto dall'operatore di back office.
+Il documento sarà sottoposto nuovamente al medico nella sua worklist di lavoro
+che lo modifica(prendendo atto delle correzioni).
+Verrà messo in coda di invio per il gateway.
+La firma digitale del documento sarà nuovamente applicata dal medico.
+Il documento verrà poi messo in coda di invio per l'fse e verrà inviato successivamte.</t>
+  </si>
+  <si>
+    <t>Viene gestito in back office.
+L'errore verrà corretto dall'operatore di back office.
+Il documento sarà sottoposto nuovamente al medico nella sua worklist di lavoro
+che lo modifica(prendendo atto delle correzioni).
+Verrà messo in coda di invio per il gateway.
+La firma digitale del documento sarà nuovamente applicata dal medico.
+Il documento verrà poi messo in coda di invio per l'fse e verrà inviato successivamente</t>
+  </si>
+  <si>
+    <t>Viene gestito in back office.
+Cancellando il dato errato.
+Il documento sarà sottoposto nuovamente al medico nella sua worklist di lavoro
+che lo modifica(prendendo atto delle correzioni). In questo caso specifico la mancanza del dato forzerà il medico ad inserire il nuovo valore tra un lista di possibili scelte, verrà anche indicato quale valore aveva precedentemente inserito segnalandolo come non compatibile .
+Verrà messo in coda di invio per il gateway.
+La firma digitale del documento sarà nuovamente applicata dal medico.
+Il documento verrà poi messo in coda di invio per l'fse e verrà inviato successivamente</t>
+  </si>
+  <si>
+    <t>Viene gestito in back office.
+L'errore verrà corretto dall'operatore di back office.
+L'operatore rieseguirà manualmente l'operazione di retry.</t>
   </si>
 </sst>
 </file>
@@ -3877,10 +3906,10 @@
   <dimension ref="A1:T652"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="K33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="I13" sqref="I13"/>
+      <selection pane="bottomRight" activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4116,7 +4145,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="150.75" thickBot="1">
+    <row r="9" spans="1:20" ht="285.75" thickBot="1">
       <c r="A9" s="20">
         <v>32</v>
       </c>
@@ -4161,7 +4190,7 @@
         <v>60</v>
       </c>
       <c r="P9" s="25" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="Q9" s="25" t="s">
         <v>158</v>
@@ -4172,7 +4201,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="165.75" thickBot="1">
+    <row r="10" spans="1:20" ht="285.75" thickBot="1">
       <c r="A10" s="20">
         <v>40</v>
       </c>
@@ -4217,7 +4246,7 @@
         <v>60</v>
       </c>
       <c r="P10" s="25" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="Q10" s="25" t="s">
         <v>158</v>
@@ -4228,7 +4257,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="60.75" thickBot="1">
+    <row r="11" spans="1:20" ht="90.75" thickBot="1">
       <c r="A11" s="20">
         <v>48</v>
       </c>
@@ -4263,7 +4292,7 @@
         <v>60</v>
       </c>
       <c r="P11" s="25" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="Q11" s="25" t="s">
         <v>158</v>
@@ -4296,13 +4325,13 @@
         <v>45062</v>
       </c>
       <c r="G12" s="24" t="s">
+        <v>231</v>
+      </c>
+      <c r="H12" s="24" t="s">
         <v>232</v>
       </c>
-      <c r="H12" s="24" t="s">
+      <c r="I12" s="24" t="s">
         <v>233</v>
-      </c>
-      <c r="I12" s="24" t="s">
-        <v>234</v>
       </c>
       <c r="J12" s="25" t="s">
         <v>60</v>
@@ -4442,7 +4471,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="135.75" thickBot="1">
+    <row r="16" spans="1:20" ht="405.75" thickBot="1">
       <c r="A16" s="20">
         <v>151</v>
       </c>
@@ -4487,7 +4516,7 @@
         <v>60</v>
       </c>
       <c r="P16" s="25" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="Q16" s="25" t="s">
         <v>158</v>
@@ -4498,7 +4527,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="135.75" thickBot="1">
+    <row r="17" spans="1:20" ht="285.75" thickBot="1">
       <c r="A17" s="20">
         <v>152</v>
       </c>
@@ -4543,7 +4572,7 @@
         <v>60</v>
       </c>
       <c r="P17" s="25" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="Q17" s="25" t="s">
         <v>158</v>
@@ -4554,7 +4583,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="135.75" thickBot="1">
+    <row r="18" spans="1:20" ht="405.75" thickBot="1">
       <c r="A18" s="20">
         <v>153</v>
       </c>
@@ -4599,7 +4628,7 @@
         <v>60</v>
       </c>
       <c r="P18" s="25" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="Q18" s="25" t="s">
         <v>158</v>
@@ -4610,7 +4639,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="135.75" thickBot="1">
+    <row r="19" spans="1:20" ht="285.75" thickBot="1">
       <c r="A19" s="20">
         <v>154</v>
       </c>
@@ -4655,7 +4684,7 @@
         <v>60</v>
       </c>
       <c r="P19" s="34" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="Q19" s="34" t="s">
         <v>158</v>
@@ -4666,7 +4695,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="135.75" thickBot="1">
+    <row r="20" spans="1:20" ht="285.75" thickBot="1">
       <c r="A20" s="20">
         <v>155</v>
       </c>
@@ -4711,7 +4740,7 @@
         <v>60</v>
       </c>
       <c r="P20" s="34" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="Q20" s="34" t="s">
         <v>158</v>
@@ -4722,7 +4751,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="135.75" thickBot="1">
+    <row r="21" spans="1:20" ht="285.75" thickBot="1">
       <c r="A21" s="20">
         <v>156</v>
       </c>
@@ -4767,7 +4796,7 @@
         <v>60</v>
       </c>
       <c r="P21" s="34" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="Q21" s="34" t="s">
         <v>158</v>
@@ -4778,7 +4807,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="135.75" thickBot="1">
+    <row r="22" spans="1:20" ht="285.75" thickBot="1">
       <c r="A22" s="20">
         <v>157</v>
       </c>
@@ -4823,7 +4852,7 @@
         <v>60</v>
       </c>
       <c r="P22" s="34" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="Q22" s="34" t="s">
         <v>158</v>
@@ -4834,7 +4863,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="135.75" thickBot="1">
+    <row r="23" spans="1:20" ht="285.75" thickBot="1">
       <c r="A23" s="20">
         <v>158</v>
       </c>
@@ -4879,7 +4908,7 @@
         <v>60</v>
       </c>
       <c r="P23" s="34" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="Q23" s="34" t="s">
         <v>158</v>
@@ -4890,7 +4919,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="135.75" thickBot="1">
+    <row r="24" spans="1:20" ht="285.75" thickBot="1">
       <c r="A24" s="20">
         <v>159</v>
       </c>
@@ -4935,7 +4964,7 @@
         <v>60</v>
       </c>
       <c r="P24" s="34" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="Q24" s="34" t="s">
         <v>158</v>
@@ -4946,7 +4975,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="135.75" thickBot="1">
+    <row r="25" spans="1:20" ht="285.75" thickBot="1">
       <c r="A25" s="20">
         <v>160</v>
       </c>
@@ -4991,7 +5020,7 @@
         <v>60</v>
       </c>
       <c r="P25" s="34" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="Q25" s="34" t="s">
         <v>158</v>
@@ -5047,7 +5076,7 @@
         <v>60</v>
       </c>
       <c r="P26" s="34" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="Q26" s="34" t="s">
         <v>158</v>
@@ -5096,7 +5125,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="135.75" thickBot="1">
+    <row r="28" spans="1:20" ht="285.75" thickBot="1">
       <c r="A28" s="20">
         <v>163</v>
       </c>
@@ -5141,7 +5170,7 @@
         <v>60</v>
       </c>
       <c r="P28" s="34" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="Q28" s="34" t="s">
         <v>158</v>
@@ -5342,7 +5371,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="135">
+    <row r="34" spans="1:20" ht="285">
       <c r="A34" s="20">
         <v>169</v>
       </c>
@@ -5387,7 +5416,7 @@
         <v>60</v>
       </c>
       <c r="P34" s="34" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="Q34" s="34" t="s">
         <v>158</v>

</xml_diff>